<commit_message>
Burndown Chart Release1/Sprint 1 Updated Version
</commit_message>
<xml_diff>
--- a/BurndownChart-Grp004.xlsx
+++ b/BurndownChart-Grp004.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomwalker/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Da Bomb\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13F5195-3ED0-9348-B953-B1792DEA9412}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D391F7E-C177-42A7-856F-C429F3E34F64}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28720" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burn down chart" sheetId="2" r:id="rId1"/>
@@ -507,6 +507,30 @@
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2875,15 +2899,15 @@
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="29.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="29.83203125" style="1"/>
+    <col min="1" max="16384" width="29.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2892,7 +2916,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2903,7 +2927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -2914,25 +2938,25 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -2940,14 +2964,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -2958,7 +2982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>20</v>
       </c>
@@ -2969,122 +2993,146 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>19</v>
       </c>
       <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C14" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>18</v>
       </c>
       <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C15" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>17</v>
       </c>
       <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C16" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C17" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C18" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>14</v>
       </c>
       <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C19" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>13</v>
       </c>
       <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C20" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>12</v>
       </c>
       <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C21" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>11</v>
       </c>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>10</v>
       </c>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>9</v>
       </c>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>8</v>
       </c>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>7</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>6</v>
       </c>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>5</v>
       </c>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>4</v>
       </c>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>3</v>
       </c>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2</v>
       </c>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>1</v>
       </c>
       <c r="B32" s="3"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -3093,140 +3141,140 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D44" s="2"/>
     </row>
-    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D80" s="2"/>
     </row>
-    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D117" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Burndown Chart Release 1/Sprint 1 Updated to Day 10
</commit_message>
<xml_diff>
--- a/BurndownChart-Grp004.xlsx
+++ b/BurndownChart-Grp004.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Da Bomb\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D391F7E-C177-42A7-856F-C429F3E34F64}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50896363-84C9-4D55-A6EC-B0662EB159A5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,6 +531,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2899,7 +2902,7 @@
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3070,6 +3073,9 @@
         <v>11</v>
       </c>
       <c r="B22" s="3"/>
+      <c r="C22" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">

</xml_diff>

<commit_message>
Burndown Chart Release1/Sprint 1 Day 14
</commit_message>
<xml_diff>
--- a/BurndownChart-Grp004.xlsx
+++ b/BurndownChart-Grp004.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Da Bomb\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50896363-84C9-4D55-A6EC-B0662EB159A5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{07A92D44-62AD-4FD4-AF3F-7D3D01A8B69A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,6 +534,15 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2902,7 +2911,7 @@
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3082,24 +3091,36 @@
         <v>10</v>
       </c>
       <c r="B23" s="3"/>
+      <c r="C23" s="1">
+        <v>18</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>9</v>
       </c>
       <c r="B24" s="3"/>
+      <c r="C24" s="1">
+        <v>17</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>8</v>
       </c>
       <c r="B25" s="3"/>
+      <c r="C25" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>7</v>
       </c>
       <c r="B26" s="3"/>
+      <c r="C26" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">

</xml_diff>

<commit_message>
Burndown Chart Release 1/ Sprint 1 Day 18
</commit_message>
<xml_diff>
--- a/BurndownChart-Grp004.xlsx
+++ b/BurndownChart-Grp004.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Da Bomb\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07A92D44-62AD-4FD4-AF3F-7D3D01A8B69A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9C26E48-0566-4006-B58E-73BF6C43871E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,6 +85,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -101,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -115,6 +121,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -161,722 +168,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-AU"/>
-              <a:t>Sprint 1 Burn</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> Down C</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU"/>
-              <a:t>hart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Burn down chart'!$B$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal Tasks Remaining</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Burn down chart'!$A$13:$A$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Burn down chart'!$B$13:$B$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-420C-4A71-9971-542ECB6C951A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Burn down chart'!$C$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Actual Tasks Remaining</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Burn down chart'!$A$13:$A$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Burn down chart'!$C$13:$C$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-420C-4A71-9971-542ECB6C951A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="590107240"/>
-        <c:axId val="590108552"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="590107240"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU"/>
-                  <a:t>Days</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t> Remaning</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-AU"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="590108552"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="590108552"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU"/>
-                  <a:t>Tasks</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t> Remaining</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-AU"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="590107240"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst>
-      <a:outerShdw dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
-        <a:srgbClr val="000000">
-          <a:alpha val="43137"/>
-        </a:srgbClr>
-      </a:outerShdw>
-    </a:effectLst>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1452,6 +743,603 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 1 Burn Down Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Tasks Remaining</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Burn down chart'!$A$13:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burn down chart'!$B$13:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A57A-4FC0-BB6E-806C05F4D314}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Tasks Remaining</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Burn down chart'!$A$13:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burn down chart'!$C$13:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A57A-4FC0-BB6E-806C05F4D314}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="609684184"/>
+        <c:axId val="609687464"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="609684184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="609687464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="609687464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="609684184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2049,7 +1937,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2157,11 +2045,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2172,11 +2055,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2208,9 +2086,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2566,44 +2441,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>381001</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1133475</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -2629,6 +2466,42 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>158751</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>148430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>448470</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>39688</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA6E9C86-AF6E-4CB9-86FF-8DE74F6ACD89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2910,8 +2783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3009,7 +2882,7 @@
       <c r="A14" s="1">
         <v>19</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="1">
         <v>35</v>
       </c>
@@ -3018,7 +2891,7 @@
       <c r="A15" s="1">
         <v>18</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="1">
         <v>33</v>
       </c>
@@ -3027,7 +2900,7 @@
       <c r="A16" s="1">
         <v>17</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="1">
         <v>30</v>
       </c>
@@ -3036,7 +2909,7 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="1">
         <v>26</v>
       </c>
@@ -3045,7 +2918,7 @@
       <c r="A18" s="1">
         <v>15</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="1">
         <v>26</v>
       </c>
@@ -3054,7 +2927,7 @@
       <c r="A19" s="1">
         <v>14</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="1">
         <v>24</v>
       </c>
@@ -3063,7 +2936,7 @@
       <c r="A20" s="1">
         <v>13</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="1">
         <v>24</v>
       </c>
@@ -3072,7 +2945,7 @@
       <c r="A21" s="1">
         <v>12</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="1">
         <v>24</v>
       </c>
@@ -3081,7 +2954,7 @@
       <c r="A22" s="1">
         <v>11</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="1">
         <v>20</v>
       </c>
@@ -3090,7 +2963,7 @@
       <c r="A23" s="1">
         <v>10</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="1">
         <v>18</v>
       </c>
@@ -3099,7 +2972,7 @@
       <c r="A24" s="1">
         <v>9</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="1">
         <v>17</v>
       </c>
@@ -3108,7 +2981,7 @@
       <c r="A25" s="1">
         <v>8</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="1">
         <v>16</v>
       </c>
@@ -3117,7 +2990,7 @@
       <c r="A26" s="1">
         <v>7</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="1">
         <v>14</v>
       </c>
@@ -3126,37 +2999,52 @@
       <c r="A27" s="1">
         <v>6</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>5</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>4</v>
       </c>
-      <c r="B29" s="3"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>3</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2</v>
       </c>
-      <c r="B31" s="3"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>1</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="7"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Final Sprint 1 Burndown And Release Update
</commit_message>
<xml_diff>
--- a/BurndownChart-Grp004.xlsx
+++ b/BurndownChart-Grp004.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Da Bomb\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9C26E48-0566-4006-B58E-73BF6C43871E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212F012C-E368-4737-81CD-FB2DB559BD53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burn down chart" sheetId="2" r:id="rId1"/>
@@ -112,6 +112,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -121,7 +122,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,6 +415,9 @@
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1126,6 +1129,12 @@
                 <c:pt idx="18">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2783,8 +2792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2793,13 +2802,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2828,6 +2837,9 @@
         <v>1</v>
       </c>
       <c r="B4" s="3"/>
+      <c r="C4" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -2850,11 +2862,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -2882,7 +2894,7 @@
       <c r="A14" s="1">
         <v>19</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="1">
         <v>35</v>
       </c>
@@ -2891,7 +2903,7 @@
       <c r="A15" s="1">
         <v>18</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="1">
         <v>33</v>
       </c>
@@ -2900,7 +2912,7 @@
       <c r="A16" s="1">
         <v>17</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="1">
         <v>30</v>
       </c>
@@ -2909,7 +2921,7 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="7"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="1">
         <v>26</v>
       </c>
@@ -2918,7 +2930,7 @@
       <c r="A18" s="1">
         <v>15</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="1">
         <v>26</v>
       </c>
@@ -2927,7 +2939,7 @@
       <c r="A19" s="1">
         <v>14</v>
       </c>
-      <c r="B19" s="7"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="1">
         <v>24</v>
       </c>
@@ -2936,7 +2948,7 @@
       <c r="A20" s="1">
         <v>13</v>
       </c>
-      <c r="B20" s="7"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="1">
         <v>24</v>
       </c>
@@ -2945,7 +2957,7 @@
       <c r="A21" s="1">
         <v>12</v>
       </c>
-      <c r="B21" s="7"/>
+      <c r="B21" s="4"/>
       <c r="C21" s="1">
         <v>24</v>
       </c>
@@ -2954,7 +2966,7 @@
       <c r="A22" s="1">
         <v>11</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="1">
         <v>20</v>
       </c>
@@ -2963,7 +2975,7 @@
       <c r="A23" s="1">
         <v>10</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B23" s="4"/>
       <c r="C23" s="1">
         <v>18</v>
       </c>
@@ -2972,7 +2984,7 @@
       <c r="A24" s="1">
         <v>9</v>
       </c>
-      <c r="B24" s="7"/>
+      <c r="B24" s="4"/>
       <c r="C24" s="1">
         <v>17</v>
       </c>
@@ -2981,7 +2993,7 @@
       <c r="A25" s="1">
         <v>8</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="1">
         <v>16</v>
       </c>
@@ -2990,7 +3002,7 @@
       <c r="A26" s="1">
         <v>7</v>
       </c>
-      <c r="B26" s="7"/>
+      <c r="B26" s="4"/>
       <c r="C26" s="1">
         <v>14</v>
       </c>
@@ -2999,7 +3011,7 @@
       <c r="A27" s="1">
         <v>6</v>
       </c>
-      <c r="B27" s="7"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="1">
         <v>12</v>
       </c>
@@ -3008,7 +3020,7 @@
       <c r="A28" s="1">
         <v>5</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="1">
         <v>10</v>
       </c>
@@ -3017,7 +3029,7 @@
       <c r="A29" s="1">
         <v>4</v>
       </c>
-      <c r="B29" s="7"/>
+      <c r="B29" s="4"/>
       <c r="C29" s="1">
         <v>7</v>
       </c>
@@ -3026,7 +3038,7 @@
       <c r="A30" s="1">
         <v>3</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="4"/>
       <c r="C30" s="1">
         <v>5</v>
       </c>
@@ -3035,7 +3047,7 @@
       <c r="A31" s="1">
         <v>2</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="4"/>
       <c r="C31" s="1">
         <v>2</v>
       </c>
@@ -3044,7 +3056,10 @@
       <c r="A32" s="1">
         <v>1</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -3054,6 +3069,9 @@
       <c r="B33" s="1">
         <v>0</v>
       </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -3093,9 +3111,9 @@
       <c r="D44" s="2"/>
     </row>
     <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D66" s="2"/>
@@ -3143,9 +3161,9 @@
       <c r="D80" s="2"/>
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="5"/>
+      <c r="A101" s="5"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D103" s="2"/>

</xml_diff>